<commit_message>
Add the changes made to HypothyroidismElimination file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MorbidTestData.xlsx
+++ b/src/test/resources/TestData/MorbidTestData.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="HypothyroidismRecipesWithAdd" r:id="rId3" sheetId="1"/>
     <sheet name="LunchFoodCatrecipes" r:id="rId4" sheetId="2"/>
+    <sheet name="HypothyroidismElimination" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="61">
   <si>
     <t>Recipe Id</t>
   </si>
@@ -326,6 +327,38 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/matar-ghughni-43043r</t>
+  </si>
+  <si>
+    <t>Recipe Category(Breakfast/lunch/snack/dinner)</t>
+  </si>
+  <si>
+    <t>2794</t>
+  </si>
+  <si>
+    <t>Instant Rabri, Quick Rabdi</t>
+  </si>
+  <si>
+    <t>For Instant Rabri
+3 cups full-fat milk
+2 fresh bread slices
+1 tbsp sugar
+1/2 cup condensed milk
+For The Garnish
+1/4 tsp cardamom (elaichi) powder</t>
+  </si>
+  <si>
+    <t>For instant rabri
+To make instant rabri, remove the crusts of the bread slices and discard. Grind the bread slices in a food processor to make fresh bread crumbs and keep aside.
+Bring the milk to boil in a broad non-stick pan.
+Add the fresh bread crumbs, sugar and condensed milk, mix well and cook on a medium flame for approx. 8 to 10 minutes, while stirring continuously and scrapping the sides of the pan.
+Allow the instant rabri to cool completely and refrigerate for 2 to 3 hours.
+Serve the instant rabri chilled garnished with cardamom powder.</t>
+  </si>
+  <si>
+    <t>Diabetic</t>
+  </si>
+  <si>
+    <t>https://tarladalal.com/instant-rabri-quick-rabdi-2794r</t>
   </si>
 </sst>
 </file>
@@ -1041,4 +1074,85 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="I2" s="0"/>
+      <c r="J2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a new file 'hypothyroidism'
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MorbidTestData.xlsx
+++ b/src/test/resources/TestData/MorbidTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="63">
   <si>
     <t>Recipe Id</t>
   </si>
@@ -359,6 +359,18 @@
   </si>
   <si>
     <t>https://tarladalal.com/instant-rabri-quick-rabdi-2794r</t>
+  </si>
+  <si>
+    <t>Energy 344 cal
+Protein 10.4 g
+Carbohydrates 38.3 g
+Fiber 0 g
+Fat 13.3 g
+Cholesterol 24 mg
+Sodium 79.3 mg</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
   </si>
 </sst>
 </file>
@@ -1144,9 +1156,11 @@
       <c r="H2" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="I2" s="0"/>
+      <c r="I2" t="s" s="0">
+        <v>61</v>
+      </c>
       <c r="J2" t="s" s="0">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>60</v>

</xml_diff>

<commit_message>
Added classes in testng.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MorbidTestData.xlsx
+++ b/src/test/resources/TestData/MorbidTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3738" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8140" uniqueCount="548">
   <si>
     <t>Recipe Id</t>
   </si>
@@ -1780,6 +1780,57 @@
   </si>
   <si>
     <t>quinoa</t>
+  </si>
+  <si>
+    <t>[Diabetic, PCOS, Diabetic]</t>
+  </si>
+  <si>
+    <t>[Diabetic, PCOS, Diabetic, PCOS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veg Veg </t>
+  </si>
+  <si>
+    <t>[PCOS, PCOS]</t>
+  </si>
+  <si>
+    <t>[Diabetic, Diabetic]</t>
+  </si>
+  <si>
+    <t>[Snacks, Breakfast, Snacks]</t>
+  </si>
+  <si>
+    <t>[Snacks, Breakfast, Snacks, Breakfast]</t>
+  </si>
+  <si>
+    <t>[Dinner, Lunch, Dinner]</t>
+  </si>
+  <si>
+    <t>[Dinner, Lunch, Dinner, Lunch]</t>
+  </si>
+  <si>
+    <t>[Breakfast, Breakfast]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veg Vegetarian Veg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetarian Veg Vegetarian Veg </t>
+  </si>
+  <si>
+    <t>[Snacks, Snacks]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jain Jain </t>
+  </si>
+  <si>
+    <t>[Dinner, Dinner]</t>
+  </si>
+  <si>
+    <t>[Veg, Veg]</t>
+  </si>
+  <si>
+    <t>[Veg, Veg, Veg]</t>
   </si>
 </sst>
 </file>
@@ -4466,7 +4517,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>47</v>
+        <v>547</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>57</v>
@@ -6747,7 +6798,7 @@
         <v>72</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>66</v>
+        <v>532</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>67</v>
@@ -6764,7 +6815,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>78</v>
@@ -6793,7 +6844,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>86</v>
@@ -6822,7 +6873,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>93</v>
@@ -6851,7 +6902,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>431</v>
@@ -6866,7 +6917,7 @@
         <v>432</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>201</v>
+        <v>534</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>428</v>
@@ -6912,7 +6963,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E8" t="s" s="0">
         <v>106</v>
@@ -6927,7 +6978,7 @@
         <v>108</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>52</v>
+        <v>535</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>103</v>
@@ -6970,7 +7021,7 @@
         <v>120</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>117</v>
+        <v>537</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>65</v>
@@ -7002,7 +7053,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E11" t="s" s="0">
         <v>128</v>
@@ -7028,10 +7079,10 @@
         <v>136</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>133</v>
+        <v>539</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E12" t="s" s="0">
         <v>137</v>
@@ -7060,7 +7111,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E13" t="s" s="0">
         <v>143</v>
@@ -7089,7 +7140,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E14" t="s" s="0">
         <v>150</v>
@@ -7115,7 +7166,7 @@
         <v>449</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>187</v>
+        <v>540</v>
       </c>
       <c r="D15" t="s" s="0">
         <v>65</v>
@@ -7176,7 +7227,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>153</v>
+        <v>542</v>
       </c>
       <c r="E17" t="s" s="0">
         <v>157</v>
@@ -7220,7 +7271,7 @@
         <v>165</v>
       </c>
       <c r="J18" t="s" s="0">
-        <v>52</v>
+        <v>535</v>
       </c>
       <c r="K18" t="s" s="0">
         <v>160</v>
@@ -7237,7 +7288,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E19" t="s" s="0">
         <v>170</v>
@@ -7252,7 +7303,7 @@
         <v>172</v>
       </c>
       <c r="J19" t="s" s="0">
-        <v>52</v>
+        <v>535</v>
       </c>
       <c r="K19" t="s" s="0">
         <v>167</v>
@@ -7266,10 +7317,10 @@
         <v>177</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>116</v>
+        <v>543</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>174</v>
+        <v>544</v>
       </c>
       <c r="E20" t="s" s="0">
         <v>178</v>
@@ -7295,10 +7346,10 @@
         <v>183</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>116</v>
+        <v>543</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E21" t="s" s="0">
         <v>184</v>
@@ -7324,10 +7375,10 @@
         <v>190</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>187</v>
+        <v>540</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E22" t="s" s="0">
         <v>191</v>
@@ -7353,7 +7404,7 @@
         <v>196</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>187</v>
+        <v>540</v>
       </c>
       <c r="D23" t="s" s="0">
         <v>65</v>
@@ -7400,7 +7451,7 @@
         <v>206</v>
       </c>
       <c r="J24" t="s" s="0">
-        <v>201</v>
+        <v>534</v>
       </c>
       <c r="K24" t="s" s="0">
         <v>202</v>
@@ -7417,7 +7468,7 @@
         <v>14</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E25" t="s" s="0">
         <v>211</v>
@@ -7490,7 +7541,7 @@
         <v>225</v>
       </c>
       <c r="J27" t="s" s="0">
-        <v>52</v>
+        <v>535</v>
       </c>
       <c r="K27" t="s" s="0">
         <v>221</v>
@@ -7562,7 +7613,7 @@
         <v>242</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>187</v>
+        <v>540</v>
       </c>
       <c r="D30" t="s" s="0">
         <v>65</v>
@@ -7594,7 +7645,7 @@
         <v>14</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E31" t="s" s="0">
         <v>249</v>
@@ -7620,10 +7671,10 @@
         <v>254</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>116</v>
+        <v>543</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E32" t="s" s="0">
         <v>255</v>
@@ -7652,7 +7703,7 @@
         <v>14</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E33" t="s" s="0">
         <v>261</v>
@@ -7681,7 +7732,7 @@
         <v>14</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>174</v>
+        <v>544</v>
       </c>
       <c r="E34" t="s" s="0">
         <v>267</v>
@@ -7707,10 +7758,10 @@
         <v>272</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>116</v>
+        <v>543</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E35" t="s" s="0">
         <v>273</v>
@@ -7736,7 +7787,7 @@
         <v>278</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>117</v>
+        <v>537</v>
       </c>
       <c r="D36" t="s" s="0">
         <v>65</v>
@@ -7765,7 +7816,7 @@
         <v>284</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>116</v>
+        <v>543</v>
       </c>
       <c r="D37" t="s" s="0">
         <v>65</v>
@@ -7794,7 +7845,7 @@
         <v>290</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>116</v>
+        <v>543</v>
       </c>
       <c r="D38" t="s" s="0">
         <v>65</v>
@@ -7823,7 +7874,7 @@
         <v>296</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>116</v>
+        <v>543</v>
       </c>
       <c r="D39" t="s" s="0">
         <v>65</v>
@@ -7852,7 +7903,7 @@
         <v>302</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>187</v>
+        <v>540</v>
       </c>
       <c r="D40" t="s" s="0">
         <v>65</v>
@@ -7881,7 +7932,7 @@
         <v>308</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>132</v>
+        <v>545</v>
       </c>
       <c r="D41" t="s" s="0">
         <v>65</v>
@@ -7942,7 +7993,7 @@
         <v>14</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>74</v>
+        <v>533</v>
       </c>
       <c r="E43" t="s" s="0">
         <v>321</v>

</xml_diff>